<commit_message>
note to clarify that all file types for work items are treated as 'attachments' (unlike research notes which define html, pdf etc separately)
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBB0B50-EE03-9748-985F-64B33719ECD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AFF048-3CFF-6F49-8B78-DB46689C87F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
   </bookViews>
@@ -384,9 +384,6 @@
     <t>e.g. 'work card (PDF)'</t>
   </si>
   <si>
-    <t>file name e.g. '00286-work-card.pdf'</t>
-  </si>
-  <si>
     <t>list label</t>
   </si>
   <si>
@@ -409,6 +406,9 @@
   </si>
   <si>
     <t>filename e.g. 00286-detail-001.webp</t>
+  </si>
+  <si>
+    <t>file name e.g. '00286-work-card.pdf' (all file types are treated as 'attachments')</t>
   </si>
 </sst>
 </file>
@@ -817,7 +817,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -865,7 +865,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>40</v>
@@ -1187,7 +1187,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>104</v>
@@ -1202,7 +1202,7 @@
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>61</v>
@@ -1235,7 +1235,7 @@
         <v>16</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>64</v>
@@ -1317,10 +1317,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1332,7 +1332,7 @@
         <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1344,10 +1344,10 @@
         <v>16</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1362,7 +1362,7 @@
         <v>113</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1566,7 +1566,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:E1048576"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -1648,7 +1648,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
stable pre- incorporating themes
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C379724-714B-B446-9BB5-31038C8D6207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF460DE4-F7E5-B648-93F5-C394A5AB4667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="1" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="3" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
@@ -1551,8 +1551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A006D3C4-93E9-0943-8732-0CF384DB2AB6}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C52" sqref="C52"/>
@@ -1562,7 +1562,7 @@
   <cols>
     <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="72.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
     <col min="6" max="7" width="20.83203125" style="1" customWidth="1"/>
@@ -4131,7 +4131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A307C2-25E9-AF4C-9C45-B37330E6C0EA}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
works can now belong to series, and series can be attached to a theme
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF460DE4-F7E5-B648-93F5-C394A5AB4667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E3F2D1-E5CE-B746-AE35-72B76BCA171C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="3" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
+    <workbookView xWindow="-20" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="5" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
     <sheet name="Works" sheetId="2" r:id="rId2"/>
     <sheet name="WorkImages" sheetId="3" r:id="rId3"/>
     <sheet name="WorkAttachments" sheetId="5" r:id="rId4"/>
-    <sheet name="lookups" sheetId="4" r:id="rId5"/>
+    <sheet name="Series" sheetId="9" r:id="rId5"/>
+    <sheet name="Themes" sheetId="6" r:id="rId6"/>
+    <sheet name="ThemeSeries" sheetId="7" r:id="rId7"/>
+    <sheet name="lookups" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="195">
   <si>
     <t>Column name</t>
   </si>
@@ -601,6 +604,30 @@
   </si>
   <si>
     <t>00339</t>
+  </si>
+  <si>
+    <t>theme_id</t>
+  </si>
+  <si>
+    <t>curve-poems</t>
+  </si>
+  <si>
+    <t>theme_title</t>
+  </si>
+  <si>
+    <t>theme_date</t>
+  </si>
+  <si>
+    <t>theme_prose_key</t>
+  </si>
+  <si>
+    <t>series_id</t>
+  </si>
+  <si>
+    <t>series_title</t>
+  </si>
+  <si>
+    <t>curve-poems-series</t>
   </si>
 </sst>
 </file>
@@ -659,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -669,6 +696,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1126,7 +1156,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="b">
         <f>NOT(ISERROR(HLOOKUP(B9,Works!$1:$1,1,FALSE)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -1555,7 +1585,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -1591,7 +1621,7 @@
         <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>6</v>
+        <v>192</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>76</v>
@@ -1647,7 +1677,7 @@
         <v>2024</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>91</v>
@@ -1691,7 +1721,7 @@
         <v>2024</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>91</v>
@@ -1735,7 +1765,7 @@
         <v>2024</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>91</v>
@@ -1779,7 +1809,7 @@
         <v>2024</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>91</v>
@@ -1823,7 +1853,7 @@
         <v>2024</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>91</v>
@@ -1867,7 +1897,7 @@
         <v>2024</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>91</v>
@@ -1911,7 +1941,7 @@
         <v>2024</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>91</v>
@@ -1955,7 +1985,7 @@
         <v>2024</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>91</v>
@@ -1999,7 +2029,7 @@
         <v>2024</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>91</v>
@@ -2043,7 +2073,7 @@
         <v>2024</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>91</v>
@@ -2087,7 +2117,7 @@
         <v>2024</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>91</v>
@@ -2131,7 +2161,7 @@
         <v>2024</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>91</v>
@@ -2175,7 +2205,7 @@
         <v>2024</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>91</v>
@@ -2219,7 +2249,7 @@
         <v>2024</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>91</v>
@@ -2263,7 +2293,7 @@
         <v>2024</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>91</v>
@@ -2307,7 +2337,7 @@
         <v>2024</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>91</v>
@@ -2351,7 +2381,7 @@
         <v>2024</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>91</v>
@@ -2395,7 +2425,7 @@
         <v>2024</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>91</v>
@@ -2439,7 +2469,7 @@
         <v>2024</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>91</v>
@@ -2483,7 +2513,7 @@
         <v>2024</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>91</v>
@@ -2527,7 +2557,7 @@
         <v>2024</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>91</v>
@@ -2571,7 +2601,7 @@
         <v>2024</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>91</v>
@@ -2615,7 +2645,7 @@
         <v>2024</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>91</v>
@@ -2659,7 +2689,7 @@
         <v>2024</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>91</v>
@@ -2703,7 +2733,7 @@
         <v>2024</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>91</v>
@@ -2747,7 +2777,7 @@
         <v>2024</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>91</v>
@@ -2791,7 +2821,7 @@
         <v>2024</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>91</v>
@@ -2835,7 +2865,7 @@
         <v>2024</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>91</v>
@@ -2879,7 +2909,7 @@
         <v>2024</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>91</v>
@@ -2923,7 +2953,7 @@
         <v>2024</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>91</v>
@@ -2967,7 +2997,7 @@
         <v>2024</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>91</v>
@@ -3011,7 +3041,7 @@
         <v>2024</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>91</v>
@@ -3055,7 +3085,7 @@
         <v>2024</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>91</v>
@@ -3099,7 +3129,7 @@
         <v>2024</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>91</v>
@@ -3143,7 +3173,7 @@
         <v>2024</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>91</v>
@@ -3187,7 +3217,7 @@
         <v>2024</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>91</v>
@@ -3231,7 +3261,7 @@
         <v>2024</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>91</v>
@@ -3275,7 +3305,7 @@
         <v>2024</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>91</v>
@@ -3319,7 +3349,7 @@
         <v>2024</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>91</v>
@@ -3363,7 +3393,7 @@
         <v>2024</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>91</v>
@@ -3407,7 +3437,7 @@
         <v>2024</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>91</v>
@@ -3451,7 +3481,7 @@
         <v>2024</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>91</v>
@@ -3495,7 +3525,7 @@
         <v>2024</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>91</v>
@@ -3539,7 +3569,7 @@
         <v>2024</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>91</v>
@@ -3583,7 +3613,7 @@
         <v>2024</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>91</v>
@@ -3627,7 +3657,7 @@
         <v>2024</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>91</v>
@@ -3671,7 +3701,7 @@
         <v>2024</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>91</v>
@@ -3715,7 +3745,7 @@
         <v>2024</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>91</v>
@@ -3759,7 +3789,7 @@
         <v>2024</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>91</v>
@@ -3803,7 +3833,7 @@
         <v>2024</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>91</v>
@@ -3847,7 +3877,7 @@
         <v>2024</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>91</v>
@@ -3891,7 +3921,7 @@
         <v>2024</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>91</v>
@@ -3935,7 +3965,7 @@
         <v>2024</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>91</v>
@@ -3979,7 +4009,7 @@
         <v>2024</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>91</v>
@@ -4023,7 +4053,7 @@
         <v>2024</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>85</v>
+        <v>194</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>91</v>
@@ -4131,7 +4161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A307C2-25E9-AF4C-9C45-B37330E6C0EA}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -4177,6 +4207,135 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9B8475-BE87-C444-A643-36F19988A384}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8090762-04EB-FC46-90C1-9A8DE33FBED9}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="20.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="8">
+        <v>46046</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D2348F-09E6-1C4F-A712-D75D02A09D8F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC30609-FE54-1C46-AE81-1F762FADE82A}">
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>

</xml_diff>

<commit_message>
attachments now called files, removed WorksImages (work 'details' not supported, use file instead e.g. a pdf)
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18252E2D-5071-4A4D-A946-DB738F2AC2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C33C27-35C3-5F4C-BDFC-84B50007EC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="1" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="2" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
     <sheet name="Works" sheetId="2" r:id="rId2"/>
-    <sheet name="WorkImages" sheetId="3" r:id="rId3"/>
+    <sheet name="WorkFiles" sheetId="10" r:id="rId3"/>
     <sheet name="WorkAttachments" sheetId="5" r:id="rId4"/>
     <sheet name="Series" sheetId="9" r:id="rId5"/>
     <sheet name="Themes" sheetId="6" r:id="rId6"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="193">
   <si>
     <t>Column name</t>
   </si>
@@ -231,12 +231,6 @@
     <t>join supplemental images to a work page.</t>
   </si>
   <si>
-    <t>detail | wip | install | alternate</t>
-  </si>
-  <si>
-    <t>consistent meaning and optional grouping on the work page.</t>
-  </si>
-  <si>
     <t>not derived from other fields, leave work-specific and follow master image naming</t>
   </si>
   <si>
@@ -342,21 +336,9 @@
     <t>001</t>
   </si>
   <si>
-    <t>detail</t>
-  </si>
-  <si>
     <t>reference for image rows; debugging, curation, sorting</t>
   </si>
   <si>
-    <t>00286-detail-001.webp</t>
-  </si>
-  <si>
-    <t>Detail 1</t>
-  </si>
-  <si>
-    <t>Detail 1 of work 00286</t>
-  </si>
-  <si>
     <t>00286-work-card.pdf</t>
   </si>
   <si>
@@ -628,6 +610,18 @@
   </si>
   <si>
     <t>curves</t>
+  </si>
+  <si>
+    <t>detail | work in progress | installation</t>
+  </si>
+  <si>
+    <t>consistent meaning and optional grouping of images on the work page.</t>
+  </si>
+  <si>
+    <t>file_id</t>
+  </si>
+  <si>
+    <t>file_label</t>
   </si>
 </sst>
 </file>
@@ -686,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -696,9 +690,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1087,7 +1078,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>40</v>
@@ -1099,13 +1090,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1165,7 +1156,7 @@
         <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1174,16 +1165,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1192,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>59</v>
@@ -1210,7 +1201,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>60</v>
@@ -1270,7 +1261,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>44</v>
@@ -1303,7 +1294,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>36</v>
@@ -1321,7 +1312,7 @@
         <v>56</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>57</v>
@@ -1387,29 +1378,29 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B26,WorkImages!$1:$1,1,FALSE)))</f>
-        <v>1</v>
+        <f>NOT(ISERROR(HLOOKUP(B26,#REF!,1,FALSE)))</f>
+        <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B27,WorkImages!$1:$1,1,FALSE)))</f>
-        <v>1</v>
+        <f>NOT(ISERROR(HLOOKUP(B27,#REF!,1,FALSE)))</f>
+        <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>61</v>
@@ -1417,41 +1408,41 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B28,WorkImages!$1:$1,1,FALSE)))</f>
-        <v>1</v>
+        <f>NOT(ISERROR(HLOOKUP(B28,#REF!,1,FALSE)))</f>
+        <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>62</v>
+        <v>189</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B29,WorkImages!$1:$1,1,FALSE)))</f>
-        <v>1</v>
+        <f>NOT(ISERROR(HLOOKUP(B29,#REF!,1,FALSE)))</f>
+        <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B30,WorkImages!$1:$1,1,FALSE)))</f>
-        <v>1</v>
+        <f>NOT(ISERROR(HLOOKUP(B30,#REF!,1,FALSE)))</f>
+        <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>17</v>
@@ -1460,62 +1451,62 @@
         <v>25</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B31,WorkImages!$1:$1,1,FALSE)))</f>
-        <v>1</v>
+        <f>NOT(ISERROR(HLOOKUP(B31,#REF!,1,FALSE)))</f>
+        <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B32,WorkImages!$1:$1,1,FALSE)))</f>
-        <v>1</v>
+        <f>NOT(ISERROR(HLOOKUP(B32,#REF!,1,FALSE)))</f>
+        <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="b">
-        <f>NOT(ISERROR(HLOOKUP(B33,WorkImages!$1:$1,1,FALSE)))</f>
-        <v>1</v>
+        <f>NOT(ISERROR(HLOOKUP(B33,#REF!,1,FALSE)))</f>
+        <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1524,10 +1515,10 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1539,7 +1530,7 @@
         <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1551,10 +1542,10 @@
         <v>16</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1563,13 +1554,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1581,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A006D3C4-93E9-0943-8732-0CF384DB2AB6}">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
@@ -1592,7 +1583,7 @@
   <cols>
     <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="72.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
     <col min="6" max="7" width="20.83203125" style="1" customWidth="1"/>
@@ -1609,7 +1600,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
@@ -1621,13 +1612,13 @@
         <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>24</v>
@@ -1662,13 +1653,13 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1">
         <v>2024</v>
@@ -1677,16 +1668,16 @@
         <v>2024</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K2" s="1">
         <v>42</v>
@@ -1695,24 +1686,24 @@
         <v>29.7</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O2" s="8">
         <v>46046</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D3" s="1">
         <v>2024</v>
@@ -1721,16 +1712,16 @@
         <v>2024</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K3" s="1">
         <v>29.7</v>
@@ -1739,42 +1730,42 @@
         <v>42</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O3" s="8">
         <v>46046</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K4" s="1">
         <v>42</v>
@@ -1783,42 +1774,42 @@
         <v>29.7</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O4" s="8">
         <v>46046</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K5" s="1">
         <v>42</v>
@@ -1827,42 +1818,42 @@
         <v>29.7</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O5" s="8">
         <v>46046</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K6" s="1">
         <v>42</v>
@@ -1871,42 +1862,42 @@
         <v>29.7</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O6" s="8">
         <v>46046</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J7" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K7" s="1">
         <v>42</v>
@@ -1915,42 +1906,42 @@
         <v>29.7</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O7" s="8">
         <v>46046</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J8" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K8" s="1">
         <v>42</v>
@@ -1959,24 +1950,24 @@
         <v>29.7</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O8" s="8">
         <v>46046</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1">
         <v>2024</v>
@@ -1985,16 +1976,16 @@
         <v>2024</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K9" s="1">
         <v>42</v>
@@ -2003,24 +1994,24 @@
         <v>29.7</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O9" s="8">
         <v>46046</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D10" s="1">
         <v>2024</v>
@@ -2029,16 +2020,16 @@
         <v>2024</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K10" s="1">
         <v>42</v>
@@ -2047,24 +2038,24 @@
         <v>29.7</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O10" s="8">
         <v>46046</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D11" s="1">
         <v>2024</v>
@@ -2073,16 +2064,16 @@
         <v>2024</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K11" s="1">
         <v>42</v>
@@ -2091,24 +2082,24 @@
         <v>29.7</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O11" s="8">
         <v>46046</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D12" s="1">
         <v>2024</v>
@@ -2117,16 +2108,16 @@
         <v>2024</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K12" s="1">
         <v>42</v>
@@ -2135,24 +2126,24 @@
         <v>29.7</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O12" s="8">
         <v>46046</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D13" s="1">
         <v>2024</v>
@@ -2161,16 +2152,16 @@
         <v>2024</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K13" s="1">
         <v>42</v>
@@ -2179,24 +2170,24 @@
         <v>29.7</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O13" s="8">
         <v>46046</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14" s="1">
         <v>2024</v>
@@ -2205,16 +2196,16 @@
         <v>2024</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K14" s="1">
         <v>42</v>
@@ -2223,24 +2214,24 @@
         <v>29.7</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O14" s="8">
         <v>46046</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D15" s="1">
         <v>2024</v>
@@ -2249,16 +2240,16 @@
         <v>2024</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K15" s="1">
         <v>42</v>
@@ -2267,24 +2258,24 @@
         <v>29.7</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O15" s="8">
         <v>46046</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D16" s="1">
         <v>2024</v>
@@ -2293,16 +2284,16 @@
         <v>2024</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K16" s="1">
         <v>42</v>
@@ -2311,24 +2302,24 @@
         <v>29.7</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O16" s="8">
         <v>46046</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="1">
         <v>2024</v>
@@ -2337,16 +2328,16 @@
         <v>2024</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K17" s="1">
         <v>42</v>
@@ -2355,24 +2346,24 @@
         <v>29.7</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O17" s="8">
         <v>46046</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D18" s="1">
         <v>2024</v>
@@ -2381,16 +2372,16 @@
         <v>2024</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K18" s="1">
         <v>42</v>
@@ -2399,42 +2390,42 @@
         <v>29.7</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O18" s="8">
         <v>46046</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E19" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J19" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K19" s="1">
         <v>42</v>
@@ -2443,42 +2434,42 @@
         <v>29.7</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O19" s="8">
         <v>46046</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E20" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J20" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K20" s="1">
         <v>42</v>
@@ -2487,42 +2478,42 @@
         <v>29.7</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O20" s="8">
         <v>46046</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E21" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J21" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K21" s="1">
         <v>42</v>
@@ -2531,42 +2522,42 @@
         <v>29.7</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O21" s="8">
         <v>46046</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J22" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K22" s="1">
         <v>42</v>
@@ -2575,24 +2566,24 @@
         <v>29.7</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O22" s="8">
         <v>46046</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" s="1">
         <v>2024</v>
@@ -2601,16 +2592,16 @@
         <v>2024</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K23" s="1">
         <v>42</v>
@@ -2619,24 +2610,24 @@
         <v>29.7</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O23" s="8">
         <v>46046</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D24" s="1">
         <v>2024</v>
@@ -2645,16 +2636,16 @@
         <v>2024</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K24" s="1">
         <v>42</v>
@@ -2663,42 +2654,42 @@
         <v>29.7</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O24" s="8">
         <v>46046</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D25" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E25" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J25" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K25" s="1">
         <v>42</v>
@@ -2707,42 +2698,42 @@
         <v>29.7</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O25" s="8">
         <v>46046</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E26" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J26" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K26" s="1">
         <v>42</v>
@@ -2751,24 +2742,24 @@
         <v>29.7</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O26" s="8">
         <v>46046</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D27" s="1">
         <v>2024</v>
@@ -2777,16 +2768,16 @@
         <v>2024</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K27" s="1">
         <v>42</v>
@@ -2795,42 +2786,42 @@
         <v>29.7</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O27" s="8">
         <v>46046</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E28" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J28" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K28" s="1">
         <v>42</v>
@@ -2839,24 +2830,24 @@
         <v>29.7</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O28" s="8">
         <v>46046</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D29" s="1">
         <v>2024</v>
@@ -2865,16 +2856,16 @@
         <v>2024</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K29" s="1">
         <v>42</v>
@@ -2883,42 +2874,42 @@
         <v>29.7</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O29" s="8">
         <v>46046</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E30" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J30" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K30" s="1">
         <v>42</v>
@@ -2927,24 +2918,24 @@
         <v>29.7</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O30" s="8">
         <v>46046</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D31" s="1">
         <v>2024</v>
@@ -2953,16 +2944,16 @@
         <v>2024</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K31" s="1">
         <v>42</v>
@@ -2971,42 +2962,42 @@
         <v>29.7</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O31" s="8">
         <v>46046</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E32" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J32" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K32" s="1">
         <v>42</v>
@@ -3015,42 +3006,42 @@
         <v>29.7</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O32" s="8">
         <v>46046</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D33" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E33" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J33" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K33" s="1">
         <v>42</v>
@@ -3059,42 +3050,42 @@
         <v>29.7</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O33" s="8">
         <v>46046</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E34" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J34" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K34" s="1">
         <v>42</v>
@@ -3103,24 +3094,24 @@
         <v>29.7</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O34" s="8">
         <v>46046</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D35" s="1">
         <v>2024</v>
@@ -3129,16 +3120,16 @@
         <v>2024</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K35" s="1">
         <v>42</v>
@@ -3147,24 +3138,24 @@
         <v>29.7</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O35" s="8">
         <v>46046</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D36" s="1">
         <v>2024</v>
@@ -3173,16 +3164,16 @@
         <v>2024</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K36" s="1">
         <v>42</v>
@@ -3191,24 +3182,24 @@
         <v>29.7</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O36" s="8">
         <v>46046</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D37" s="1">
         <v>2024</v>
@@ -3217,16 +3208,16 @@
         <v>2024</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K37" s="1">
         <v>42</v>
@@ -3235,24 +3226,24 @@
         <v>29.7</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O37" s="8">
         <v>46046</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D38" s="1">
         <v>2024</v>
@@ -3261,16 +3252,16 @@
         <v>2024</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K38" s="1">
         <v>42</v>
@@ -3279,24 +3270,24 @@
         <v>29.7</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O38" s="8">
         <v>46046</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D39" s="1">
         <v>2024</v>
@@ -3305,16 +3296,16 @@
         <v>2024</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K39" s="1">
         <v>42</v>
@@ -3323,24 +3314,24 @@
         <v>29.7</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O39" s="8">
         <v>46046</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D40" s="1">
         <v>2024</v>
@@ -3349,16 +3340,16 @@
         <v>2024</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K40" s="1">
         <v>42</v>
@@ -3367,24 +3358,24 @@
         <v>29.7</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O40" s="8">
         <v>46046</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D41" s="1">
         <v>2024</v>
@@ -3393,16 +3384,16 @@
         <v>2024</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K41" s="1">
         <v>42</v>
@@ -3411,24 +3402,24 @@
         <v>29.7</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O41" s="8">
         <v>46046</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D42" s="1">
         <v>2024</v>
@@ -3437,16 +3428,16 @@
         <v>2024</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K42" s="1">
         <v>42</v>
@@ -3455,42 +3446,42 @@
         <v>29.7</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O42" s="8">
         <v>46046</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D43" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E43" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J43" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K43" s="1">
         <v>42</v>
@@ -3499,24 +3490,24 @@
         <v>29.7</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O43" s="8">
         <v>46046</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D44" s="1">
         <v>2024</v>
@@ -3525,16 +3516,16 @@
         <v>2024</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K44" s="1">
         <v>42</v>
@@ -3543,24 +3534,24 @@
         <v>29.7</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O44" s="8">
         <v>46046</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D45" s="1">
         <v>2024</v>
@@ -3569,16 +3560,16 @@
         <v>2024</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K45" s="1">
         <v>42</v>
@@ -3587,24 +3578,24 @@
         <v>29.7</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O45" s="8">
         <v>46046</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D46" s="1">
         <v>2024</v>
@@ -3613,16 +3604,16 @@
         <v>2024</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K46" s="1">
         <v>42</v>
@@ -3631,24 +3622,24 @@
         <v>29.7</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O46" s="8">
         <v>46046</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D47" s="1">
         <v>2024</v>
@@ -3657,16 +3648,16 @@
         <v>2024</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K47" s="1">
         <v>42</v>
@@ -3675,24 +3666,24 @@
         <v>29.7</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O47" s="8">
         <v>46046</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D48" s="1">
         <v>2024</v>
@@ -3701,16 +3692,16 @@
         <v>2024</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K48" s="1">
         <v>42</v>
@@ -3719,24 +3710,24 @@
         <v>29.7</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O48" s="8">
         <v>46046</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D49" s="1">
         <v>2024</v>
@@ -3745,16 +3736,16 @@
         <v>2024</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K49" s="1">
         <v>42</v>
@@ -3763,24 +3754,24 @@
         <v>29.7</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O49" s="8">
         <v>46046</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D50" s="1">
         <v>2024</v>
@@ -3789,16 +3780,16 @@
         <v>2024</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K50" s="1">
         <v>42</v>
@@ -3807,24 +3798,24 @@
         <v>29.7</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O50" s="8">
         <v>46046</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D51" s="1">
         <v>2024</v>
@@ -3833,16 +3824,16 @@
         <v>2024</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K51" s="1">
         <v>42</v>
@@ -3851,24 +3842,24 @@
         <v>29.7</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O51" s="8">
         <v>46046</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D52" s="1">
         <v>2024</v>
@@ -3877,16 +3868,16 @@
         <v>2024</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K52" s="1">
         <v>42</v>
@@ -3895,24 +3886,24 @@
         <v>29.7</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O52" s="8">
         <v>46046</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D53" s="1">
         <v>2024</v>
@@ -3921,16 +3912,16 @@
         <v>2024</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K53" s="1">
         <v>42</v>
@@ -3939,24 +3930,24 @@
         <v>29.7</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O53" s="8">
         <v>46046</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D54" s="1">
         <v>2024</v>
@@ -3965,16 +3956,16 @@
         <v>2024</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K54" s="1">
         <v>42</v>
@@ -3983,42 +3974,42 @@
         <v>29.7</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O54" s="8">
         <v>46046</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B55" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D55" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E55" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J55" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K55" s="1">
         <v>42</v>
@@ -4027,42 +4018,42 @@
         <v>29.7</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O55" s="8">
         <v>46046</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B56" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E56" s="1">
+        <v>2024</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D56" s="1">
-        <v>2024</v>
-      </c>
-      <c r="E56" s="1">
-        <v>2024</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J56" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K56" s="1">
         <v>42</v>
@@ -4071,13 +4062,13 @@
         <v>29.7</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O56" s="8">
         <v>46046</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -4086,70 +4077,40 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D97D8E-FD08-1349-9CBB-22A16DB9F6B8}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FD9C38-EEDE-3B48-B7E6-A7692F053C8D}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="20.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.83203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>3</v>
+        <v>191</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>83</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4162,7 +4123,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -4175,7 +4136,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -4184,21 +4145,21 @@
         <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4228,10 +4189,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
@@ -4242,16 +4203,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" s="6">
         <v>2025</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -4279,21 +4240,21 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C2" s="8">
         <v>46051</v>
@@ -4318,25 +4279,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>191</v>
+      <c r="A1" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>188</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -4364,13 +4325,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
test print version for 286, 287
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FA6616-13A6-254E-BCB1-176AD165083E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBB8CAA-8360-714E-8F9C-AF25654CE335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="1" xr2:uid="{3340F1A4-2CEC-C74D-85F7-446226E10E48}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="379">
   <si>
     <t>Column name</t>
   </si>
@@ -1175,6 +1175,9 @@
   </si>
   <si>
     <t>ready</t>
+  </si>
+  <si>
+    <t>2017-25</t>
   </si>
 </sst>
 </file>
@@ -2055,7 +2058,7 @@
   <dimension ref="A1:X107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C58" sqref="C58"/>
@@ -7360,13 +7363,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9B8475-BE87-C444-A643-36F19988A384}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -7404,6 +7407,20 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2025</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
force generated all work, series and theme files
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501F26D5-7453-5044-AB74-39C7D7EFD38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A19190-8193-2745-928E-26226D268005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
@@ -2008,7 +2008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7389,8 +7389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added automatic deletion for draft works (for when status is changed from published -> draft)
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -492,7 +492,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col width="11.83203125" customWidth="1" style="5" min="1" max="1"/>
     <col width="24.1640625" customWidth="1" style="1" min="2" max="2"/>
@@ -1107,10 +1107,10 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col width="11.33203125" customWidth="1" style="1" min="1" max="1"/>
     <col width="34.1640625" customWidth="1" style="1" min="2" max="2"/>
@@ -1133,8 +1133,8 @@
     <col width="15.5" customWidth="1" style="1" min="22" max="22"/>
     <col width="15.1640625" customWidth="1" style="1" min="23" max="23"/>
     <col width="17.83203125" customWidth="1" style="1" min="24" max="24"/>
-    <col width="10.83203125" customWidth="1" style="1" min="25" max="25"/>
-    <col width="10.83203125" customWidth="1" style="1" min="26" max="16384"/>
+    <col width="10.83203125" customWidth="1" style="1" min="25" max="26"/>
+    <col width="10.83203125" customWidth="1" style="1" min="27" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="3">
@@ -8654,7 +8654,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col width="15.83203125" customWidth="1" min="1" max="1"/>
     <col width="24.83203125" customWidth="1" min="2" max="2"/>
@@ -8712,7 +8712,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col width="25.83203125" customWidth="1" style="1" min="1" max="1"/>
     <col width="20.83203125" customWidth="1" style="1" min="2" max="3"/>
@@ -8720,8 +8720,8 @@
     <col width="10.83203125" customWidth="1" style="1" min="5" max="5"/>
     <col width="19.83203125" customWidth="1" style="1" min="6" max="6"/>
     <col width="19" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
-    <col width="10.83203125" customWidth="1" style="1" min="8" max="8"/>
-    <col width="10.83203125" customWidth="1" style="1" min="9" max="16384"/>
+    <col width="10.83203125" customWidth="1" style="1" min="8" max="9"/>
+    <col width="10.83203125" customWidth="1" style="1" min="10" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="3">
@@ -8829,12 +8829,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col width="20.83203125" customWidth="1" style="1" min="1" max="3"/>
     <col width="17" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
-    <col width="10.83203125" customWidth="1" style="1" min="5" max="5"/>
-    <col width="10.83203125" customWidth="1" style="1" min="6" max="16384"/>
+    <col width="10.83203125" customWidth="1" style="1" min="5" max="6"/>
+    <col width="10.83203125" customWidth="1" style="1" min="7" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="3">
@@ -8899,12 +8899,12 @@
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col width="20.83203125" customWidth="1" style="1" min="1" max="1"/>
     <col width="29.6640625" customWidth="1" style="1" min="2" max="2"/>
-    <col width="10.83203125" customWidth="1" style="1" min="3" max="3"/>
-    <col width="10.83203125" customWidth="1" style="1" min="4" max="16384"/>
+    <col width="10.83203125" customWidth="1" style="1" min="3" max="4"/>
+    <col width="10.83203125" customWidth="1" style="1" min="5" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="3">

</xml_diff>

<commit_message>
removed themes from works.xlsx
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -1,31 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325BC6D1-BC13-F144-BB8A-BE9D28CCAA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3EBC4F-A010-D244-9A22-81A8BB28DDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
     <sheet name="Works" sheetId="2" r:id="rId2"/>
     <sheet name="WorkFiles" sheetId="3" r:id="rId3"/>
     <sheet name="Series" sheetId="4" r:id="rId4"/>
-    <sheet name="Themes" sheetId="5" r:id="rId5"/>
-    <sheet name="ThemeSeries" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="378">
   <si>
     <t>Works</t>
   </si>
@@ -1156,12 +1154,6 @@
   </si>
   <si>
     <t>2017-25</t>
-  </si>
-  <si>
-    <t>theme_id</t>
-  </si>
-  <si>
-    <t>curves</t>
   </si>
   <si>
     <t>curve poems (2025)</t>
@@ -2011,7 +2003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X107"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2133,7 +2125,7 @@
         <v>46055</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>85</v>
@@ -2183,7 +2175,7 @@
         <v>46055</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>93</v>
@@ -2233,7 +2225,7 @@
         <v>46055</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>96</v>
@@ -2283,7 +2275,7 @@
         <v>46055</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>98</v>
@@ -2333,7 +2325,7 @@
         <v>46055</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>100</v>
@@ -2383,7 +2375,7 @@
         <v>46055</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>102</v>
@@ -2433,7 +2425,7 @@
         <v>46055</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>104</v>
@@ -2483,7 +2475,7 @@
         <v>46055</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>107</v>
@@ -2533,7 +2525,7 @@
         <v>46055</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>110</v>
@@ -2583,7 +2575,7 @@
         <v>46055</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>113</v>
@@ -2633,7 +2625,7 @@
         <v>46055</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>116</v>
@@ -2683,7 +2675,7 @@
         <v>46055</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>118</v>
@@ -2733,7 +2725,7 @@
         <v>46055</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>120</v>
@@ -2783,7 +2775,7 @@
         <v>46055</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>122</v>
@@ -2833,7 +2825,7 @@
         <v>46055</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>124</v>
@@ -2883,7 +2875,7 @@
         <v>46055</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>126</v>
@@ -2933,7 +2925,7 @@
         <v>46055</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>128</v>
@@ -2983,7 +2975,7 @@
         <v>46055</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>130</v>
@@ -3033,7 +3025,7 @@
         <v>46055</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>132</v>
@@ -3083,7 +3075,7 @@
         <v>46055</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>134</v>
@@ -3133,7 +3125,7 @@
         <v>46055</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>136</v>
@@ -3183,7 +3175,7 @@
         <v>46055</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>138</v>
@@ -3233,7 +3225,7 @@
         <v>46055</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>141</v>
@@ -3283,7 +3275,7 @@
         <v>46055</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>143</v>
@@ -3333,7 +3325,7 @@
         <v>46055</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>145</v>
@@ -3383,7 +3375,7 @@
         <v>46055</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>147</v>
@@ -3433,7 +3425,7 @@
         <v>46055</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>149</v>
@@ -3483,7 +3475,7 @@
         <v>46055</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>151</v>
@@ -3533,7 +3525,7 @@
         <v>46055</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>153</v>
@@ -3583,7 +3575,7 @@
         <v>46055</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>156</v>
@@ -3633,7 +3625,7 @@
         <v>46055</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>158</v>
@@ -3683,7 +3675,7 @@
         <v>46055</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>160</v>
@@ -3733,7 +3725,7 @@
         <v>46055</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>163</v>
@@ -3783,7 +3775,7 @@
         <v>46055</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>166</v>
@@ -3833,7 +3825,7 @@
         <v>46055</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>168</v>
@@ -3883,7 +3875,7 @@
         <v>46055</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>170</v>
@@ -3933,7 +3925,7 @@
         <v>46055</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>173</v>
@@ -3983,7 +3975,7 @@
         <v>46055</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>175</v>
@@ -4033,7 +4025,7 @@
         <v>46055</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>178</v>
@@ -4083,7 +4075,7 @@
         <v>46055</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>180</v>
@@ -4133,7 +4125,7 @@
         <v>46055</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>182</v>
@@ -4183,7 +4175,7 @@
         <v>46055</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>184</v>
@@ -4233,7 +4225,7 @@
         <v>46055</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>186</v>
@@ -4283,7 +4275,7 @@
         <v>46055</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>188</v>
@@ -4333,7 +4325,7 @@
         <v>46055</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>190</v>
@@ -4383,7 +4375,7 @@
         <v>46055</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>192</v>
@@ -4433,7 +4425,7 @@
         <v>46055</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>194</v>
@@ -4483,7 +4475,7 @@
         <v>46055</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>196</v>
@@ -4533,7 +4525,7 @@
         <v>46055</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>198</v>
@@ -4583,7 +4575,7 @@
         <v>46055</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>200</v>
@@ -4633,7 +4625,7 @@
         <v>46055</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>202</v>
@@ -4683,7 +4675,7 @@
         <v>46055</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>204</v>
@@ -4733,7 +4725,7 @@
         <v>46055</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>206</v>
@@ -4783,7 +4775,7 @@
         <v>46055</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>208</v>
@@ -4833,7 +4825,7 @@
         <v>46055</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>211</v>
@@ -7276,7 +7268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -7397,93 +7389,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="3" width="20.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="10.83203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="8">
-        <v>46055</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.83203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated schema sheet to include 2400 flag
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDF6B7D-B4FA-BB41-BFCC-93C54B38617D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9219781F-1A43-2E42-9AD0-6AD8AA2EEBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="380">
   <si>
     <t>Works</t>
   </si>
@@ -1157,6 +1157,12 @@
   </si>
   <si>
     <t>has_primary_2400</t>
+  </si>
+  <si>
+    <t>true if not blank</t>
+  </si>
+  <si>
+    <t>generate a 2400px srcset image? (use sparingly due to large file size)</t>
   </si>
 </sst>
 </file>
@@ -1568,17 +1574,17 @@
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="54.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="85.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1695,13 +1701,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>377</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>379</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>378</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1709,13 +1715,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1723,13 +1729,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1737,13 +1743,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1751,13 +1757,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1765,13 +1771,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1779,10 +1785,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>41</v>
@@ -1793,13 +1799,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1807,10 +1813,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>46</v>
@@ -1821,13 +1827,13 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1835,13 +1841,13 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1849,13 +1855,13 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1863,13 +1869,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1877,13 +1883,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1891,13 +1897,13 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1905,13 +1911,13 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1919,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>68</v>
@@ -1933,7 +1939,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>68</v>
@@ -1942,28 +1948,28 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1971,10 +1977,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>75</v>
@@ -1985,17 +1991,32 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2003,11 +2024,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix missed series json bug, added flag to only rewrite series files (.md and .json)
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -556,7 +556,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col width="11.83203125" customWidth="1" style="5" min="1" max="1"/>
     <col width="24.1640625" customWidth="1" style="1" min="2" max="2"/>
@@ -1195,7 +1195,7 @@
       <selection pane="bottomRight" activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col width="11.33203125" customWidth="1" style="1" min="1" max="1"/>
     <col width="72.83203125" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
@@ -8761,7 +8761,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col width="25.83203125" customWidth="1" style="1" min="1" max="1"/>
     <col width="20.83203125" customWidth="1" style="1" min="2" max="3"/>
@@ -8878,7 +8878,7 @@
         </is>
       </c>
       <c r="D4" s="8" t="n">
-        <v>46066</v>
+        <v>46067</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>2021</v>
@@ -8930,7 +8930,7 @@
       <selection activeCell="A319" sqref="A319"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.83203125" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col width="41.6640625" bestFit="1" customWidth="1" style="16" min="1" max="1"/>
     <col width="9.33203125" customWidth="1" style="16" min="2" max="2"/>

</xml_diff>

<commit_message>
added moments to pipeline, with some refactoring of scripts
</commit_message>
<xml_diff>
--- a/data/works.xlsx
+++ b/data/works.xlsx
@@ -8,26 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlf/Developer/dotlineform/dotlineform-site/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA54E47B-23C8-574F-8F53-2F092C38EE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7924C44-12A3-E94C-B1AF-070B66A37613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="1" r:id="rId1"/>
     <sheet name="Works" sheetId="2" r:id="rId2"/>
     <sheet name="Series" sheetId="3" r:id="rId3"/>
     <sheet name="WorkDetails" sheetId="4" r:id="rId4"/>
-    <sheet name="index - old version" sheetId="5" r:id="rId5"/>
+    <sheet name="Moments" sheetId="6" r:id="rId5"/>
+    <sheet name="index - old version" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'index - old version'!$A$1:$G$804</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'index - old version'!$A$1:$G$804</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4724" uniqueCount="1453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5019" uniqueCount="1606">
   <si>
     <t>Works</t>
   </si>
@@ -4386,6 +4400,465 @@
   </si>
   <si>
     <t>details to publish</t>
+  </si>
+  <si>
+    <t>moment_id</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>date_display</t>
+  </si>
+  <si>
+    <t>moment_folder</t>
+  </si>
+  <si>
+    <t>13-moments-in-october</t>
+  </si>
+  <si>
+    <t>13 moments in October</t>
+  </si>
+  <si>
+    <t>4-stories</t>
+  </si>
+  <si>
+    <t>c. 2020?</t>
+  </si>
+  <si>
+    <t>4 stories</t>
+  </si>
+  <si>
+    <t>a-beautiful-route</t>
+  </si>
+  <si>
+    <t>a beautiful route</t>
+  </si>
+  <si>
+    <t>a-dance</t>
+  </si>
+  <si>
+    <t>a dance</t>
+  </si>
+  <si>
+    <t>a-doll-story</t>
+  </si>
+  <si>
+    <t>a doll story</t>
+  </si>
+  <si>
+    <t>a-feeling-of-free-will</t>
+  </si>
+  <si>
+    <t>a feeling of free will</t>
+  </si>
+  <si>
+    <t>a-lemon-tart-poem</t>
+  </si>
+  <si>
+    <t>a lemon tart poem</t>
+  </si>
+  <si>
+    <t>a-light-inside-a-flower</t>
+  </si>
+  <si>
+    <t>a light inside a flower</t>
+  </si>
+  <si>
+    <t>a-poem-about-love</t>
+  </si>
+  <si>
+    <t>c. 2018?</t>
+  </si>
+  <si>
+    <t>a poem about love</t>
+  </si>
+  <si>
+    <t>a-poem-about-purity</t>
+  </si>
+  <si>
+    <t>a poem about purity</t>
+  </si>
+  <si>
+    <t>a-question</t>
+  </si>
+  <si>
+    <t>a question</t>
+  </si>
+  <si>
+    <t>a-selina</t>
+  </si>
+  <si>
+    <t>a selina</t>
+  </si>
+  <si>
+    <t>all-the-little-cracks</t>
+  </si>
+  <si>
+    <t>c. 2015</t>
+  </si>
+  <si>
+    <t>all the little cracks</t>
+  </si>
+  <si>
+    <t>angels</t>
+  </si>
+  <si>
+    <t>c. Apr 1998</t>
+  </si>
+  <si>
+    <t>blue-sky</t>
+  </si>
+  <si>
+    <t>c. 2012?</t>
+  </si>
+  <si>
+    <t>blue sky</t>
+  </si>
+  <si>
+    <t>boundary-conditions</t>
+  </si>
+  <si>
+    <t>boundary conditions</t>
+  </si>
+  <si>
+    <t>cascading-waterfalls</t>
+  </si>
+  <si>
+    <t>c. 2016</t>
+  </si>
+  <si>
+    <t>cascading waterfalls</t>
+  </si>
+  <si>
+    <t>circle</t>
+  </si>
+  <si>
+    <t>c. 2019</t>
+  </si>
+  <si>
+    <t>clouds</t>
+  </si>
+  <si>
+    <t>c. 2019?</t>
+  </si>
+  <si>
+    <t>compiled</t>
+  </si>
+  <si>
+    <t>creatures-who-understand-light</t>
+  </si>
+  <si>
+    <t>creatures who understand light</t>
+  </si>
+  <si>
+    <t>dream-sleep</t>
+  </si>
+  <si>
+    <t>dream sleep</t>
+  </si>
+  <si>
+    <t>exit-dreams</t>
+  </si>
+  <si>
+    <t>exit dreams</t>
+  </si>
+  <si>
+    <t>healing-forms</t>
+  </si>
+  <si>
+    <t>healing forms</t>
+  </si>
+  <si>
+    <t>hi-honey</t>
+  </si>
+  <si>
+    <t>c. 2024?</t>
+  </si>
+  <si>
+    <t>hi honey</t>
+  </si>
+  <si>
+    <t>i-felt-my-self-sinking</t>
+  </si>
+  <si>
+    <t>I felt my self sinking, but not alone, and in peace</t>
+  </si>
+  <si>
+    <t>impenetrable</t>
+  </si>
+  <si>
+    <t>c. 2018</t>
+  </si>
+  <si>
+    <t>keys</t>
+  </si>
+  <si>
+    <t>leaves</t>
+  </si>
+  <si>
+    <t>little-clear-vessel</t>
+  </si>
+  <si>
+    <t>c. 1992</t>
+  </si>
+  <si>
+    <t>little clear vessel</t>
+  </si>
+  <si>
+    <t>lotus-pond</t>
+  </si>
+  <si>
+    <t>c. 2024</t>
+  </si>
+  <si>
+    <t>lotus pond</t>
+  </si>
+  <si>
+    <t>memory</t>
+  </si>
+  <si>
+    <t>occasionally</t>
+  </si>
+  <si>
+    <t>particles</t>
+  </si>
+  <si>
+    <t>c. 2013</t>
+  </si>
+  <si>
+    <t>peace-of-mind</t>
+  </si>
+  <si>
+    <t>peace of mind</t>
+  </si>
+  <si>
+    <t>perfection-of-flowers</t>
+  </si>
+  <si>
+    <t>c. 2014</t>
+  </si>
+  <si>
+    <t>perfection of flowers</t>
+  </si>
+  <si>
+    <t>rose</t>
+  </si>
+  <si>
+    <t>sadness-love</t>
+  </si>
+  <si>
+    <t>sadness love</t>
+  </si>
+  <si>
+    <t>samuel-beckett</t>
+  </si>
+  <si>
+    <t>Samuel Beckett</t>
+  </si>
+  <si>
+    <t>sleep</t>
+  </si>
+  <si>
+    <t>sleepy-moments</t>
+  </si>
+  <si>
+    <t>sleepy moments</t>
+  </si>
+  <si>
+    <t>snow</t>
+  </si>
+  <si>
+    <t>2018-2020</t>
+  </si>
+  <si>
+    <t>the-moment-collector</t>
+  </si>
+  <si>
+    <t>the moment collector</t>
+  </si>
+  <si>
+    <t>the-moon-and-the-sun</t>
+  </si>
+  <si>
+    <t>the moon and the sun</t>
+  </si>
+  <si>
+    <t>the-watch-keeper</t>
+  </si>
+  <si>
+    <t>the watch keeper</t>
+  </si>
+  <si>
+    <t>timeless</t>
+  </si>
+  <si>
+    <t>vessels</t>
+  </si>
+  <si>
+    <t>warmth</t>
+  </si>
+  <si>
+    <t>we-are-the-vessel</t>
+  </si>
+  <si>
+    <t>we are the vessel</t>
+  </si>
+  <si>
+    <t>we-make-ghosts</t>
+  </si>
+  <si>
+    <t>we make ghosts</t>
+  </si>
+  <si>
+    <t>where-words-end</t>
+  </si>
+  <si>
+    <t>where words end</t>
+  </si>
+  <si>
+    <t>where</t>
+  </si>
+  <si>
+    <t>where?</t>
+  </si>
+  <si>
+    <t>will-we-leave-residues</t>
+  </si>
+  <si>
+    <t>c. 2022</t>
+  </si>
+  <si>
+    <t>will we leave residues</t>
+  </si>
+  <si>
+    <t>winter</t>
+  </si>
+  <si>
+    <t>without-words</t>
+  </si>
+  <si>
+    <t>without words</t>
+  </si>
+  <si>
+    <t>13-moments-in-october.jpg</t>
+  </si>
+  <si>
+    <t>4-stories.jpg</t>
+  </si>
+  <si>
+    <t>a-beautiful-route.jpg</t>
+  </si>
+  <si>
+    <t>doll-glass-23.jpg</t>
+  </si>
+  <si>
+    <t>a-feeling-of-free-will.jpg</t>
+  </si>
+  <si>
+    <t>a-light-inside-a-flower.jpg</t>
+  </si>
+  <si>
+    <t>a-poem-about-love.jpg</t>
+  </si>
+  <si>
+    <t>a-poem-about-purity.jpg</t>
+  </si>
+  <si>
+    <t>all-the-little-cracks.jpg</t>
+  </si>
+  <si>
+    <t>angels.jpg</t>
+  </si>
+  <si>
+    <t>blue-sky.jpg</t>
+  </si>
+  <si>
+    <t>creatures-who-understand-light.jpg</t>
+  </si>
+  <si>
+    <t>dream-sleep.jpg</t>
+  </si>
+  <si>
+    <t>droplets.jpg</t>
+  </si>
+  <si>
+    <t>i-felt-my-self-sinking.jpg</t>
+  </si>
+  <si>
+    <t>keys.jpg</t>
+  </si>
+  <si>
+    <t>leaves.jpg</t>
+  </si>
+  <si>
+    <t>little-clear-vessel.jpg</t>
+  </si>
+  <si>
+    <t>occasionally.jpg</t>
+  </si>
+  <si>
+    <t>particles.jpg</t>
+  </si>
+  <si>
+    <t>peace-of-mind.jpg</t>
+  </si>
+  <si>
+    <t>perfection-of-flowers.jpg</t>
+  </si>
+  <si>
+    <t>samuel-beckett.jpg</t>
+  </si>
+  <si>
+    <t>sleepy-moments.jpg</t>
+  </si>
+  <si>
+    <t>snow.jpg</t>
+  </si>
+  <si>
+    <t>the-moment-collector.jpg</t>
+  </si>
+  <si>
+    <t>the-watch-keeper.jpg</t>
+  </si>
+  <si>
+    <t>warmth.jpg</t>
+  </si>
+  <si>
+    <t>we-are-the-vessel.jpg</t>
+  </si>
+  <si>
+    <t>we-make-ghosts.jpg</t>
+  </si>
+  <si>
+    <t>where-words-end.jpg</t>
+  </si>
+  <si>
+    <t>will-we-leave-residues.jpg</t>
+  </si>
+  <si>
+    <t>winter.jpg</t>
+  </si>
+  <si>
+    <t>draft</t>
+  </si>
+  <si>
+    <t>I felt my self sinking</t>
+  </si>
+  <si>
+    <t>a-lemon-tart-poem.jpg</t>
+  </si>
+  <si>
+    <t>hi-honey.jpg</t>
+  </si>
+  <si>
+    <t>impenetrable.jpg</t>
+  </si>
+  <si>
+    <t>sadness-love.jpg</t>
+  </si>
+  <si>
+    <t>moment_filename</t>
   </si>
 </sst>
 </file>
@@ -4397,7 +4870,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4458,6 +4931,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4483,7 +4970,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4522,6 +5009,17 @@
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5313,16 +5811,16 @@
   <dimension ref="A1:Y111"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A108" sqref="A108"/>
+      <selection pane="bottomRight" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="72.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -10683,8 +11181,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -10844,7 +11345,10 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -11048,13 +11552,1212 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42325F09-46A5-DE44-9D76-A93E021C1050}">
+  <dimension ref="A1:K57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" sqref="A1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="22" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.6640625" style="22" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1453</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>1454</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>1455</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>1456</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>1605</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>1457</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E2" s="23">
+        <v>45588</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>1458</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>1461</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E3" s="23">
+        <v>43831</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>1460</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E4" s="23">
+        <v>43511</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>1463</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E5" s="23">
+        <v>43215</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E6" s="23">
+        <v>45822</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>1467</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E7" s="23">
+        <v>45588</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>1469</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E8" s="23">
+        <v>44715</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>1471</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E9" s="23">
+        <v>43549</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E10" s="23">
+        <v>43101</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>1476</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E11" s="23">
+        <v>43089</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E12" s="23">
+        <v>41921</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E13" s="23">
+        <v>41875</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>1485</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E14" s="23">
+        <v>42005</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>1484</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>1485</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E15" s="23">
+        <v>35886</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>1487</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>1486</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E16" s="23">
+        <v>40909</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>1489</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>1490</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E17" s="23">
+        <v>42005</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>1484</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>1493</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E18" s="23">
+        <v>42370</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>1494</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E19" s="23">
+        <v>43466</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>1497</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E20" s="23">
+        <v>43466</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E21" s="23">
+        <v>43733</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E22" s="23">
+        <v>43466</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>1497</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>1502</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E23" s="23">
+        <v>43219</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>1504</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E24" s="23">
+        <v>42693</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>1396</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E25" s="23">
+        <v>41093</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E26" s="23">
+        <v>42528</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>1494</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E27" s="23">
+        <v>45588</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>1510</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>1511</v>
+      </c>
+      <c r="H27" s="22" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E28" s="23">
+        <v>42005</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>1484</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>1600</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E29" s="23">
+        <v>43222</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>1515</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>1514</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E30" s="23">
+        <v>43647</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>1516</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E31" s="23">
+        <v>43577</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>1517</v>
+      </c>
+      <c r="H31" s="22" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E32" s="23">
+        <v>33604</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>1519</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>1520</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E33" s="23">
+        <v>45588</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>1522</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E34" s="23">
+        <v>45878</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E35" s="23">
+        <v>43653</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>1525</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E36" s="23">
+        <v>41275</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>1527</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>1526</v>
+      </c>
+      <c r="H36" s="22" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E37" s="23">
+        <v>43704</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>1529</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E38" s="23">
+        <v>41640</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>1531</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>1532</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E39" s="23">
+        <v>43515</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E40" s="23">
+        <v>40201</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>1535</v>
+      </c>
+      <c r="H40" s="22" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E41" s="23">
+        <v>33604</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>1519</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>1537</v>
+      </c>
+      <c r="H41" s="22" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E42" s="23">
+        <v>43262</v>
+      </c>
+      <c r="G42" s="22" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E43" s="23">
+        <v>43557</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>1540</v>
+      </c>
+      <c r="H43" s="22" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E44" s="23">
+        <v>43101</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>1542</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>1541</v>
+      </c>
+      <c r="H44" s="22" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E45" s="23">
+        <v>43107</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>1544</v>
+      </c>
+      <c r="H45" s="22" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E46" s="23">
+        <v>45589</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E47" s="23">
+        <v>41667</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>1548</v>
+      </c>
+      <c r="H47" s="22" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E48" s="23">
+        <v>43221</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>1515</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E49" s="23">
+        <v>43600</v>
+      </c>
+      <c r="G49" s="22" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
+        <v>1551</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E50" s="23">
+        <v>43429</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>1551</v>
+      </c>
+      <c r="H50" s="22" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E51" s="23">
+        <v>43232</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>1553</v>
+      </c>
+      <c r="H51" s="22" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E52" s="23">
+        <v>41640</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>1531</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>1555</v>
+      </c>
+      <c r="H52" s="22" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E53" s="23">
+        <v>43226</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>1557</v>
+      </c>
+      <c r="H53" s="22" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E54" s="23">
+        <v>43648</v>
+      </c>
+      <c r="G54" s="22" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E55" s="23">
+        <v>44562</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>1561</v>
+      </c>
+      <c r="G55" s="22" t="s">
+        <v>1562</v>
+      </c>
+      <c r="H55" s="22" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
+        <v>1563</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E56" s="23">
+        <v>43236</v>
+      </c>
+      <c r="G56" s="22" t="s">
+        <v>1563</v>
+      </c>
+      <c r="H56" s="22" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>1599</v>
+      </c>
+      <c r="E57" s="23">
+        <v>43720</v>
+      </c>
+      <c r="G57" s="22" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IV840"/>
   <sheetViews>
-    <sheetView topLeftCell="A441" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A356" workbookViewId="0">
       <selection activeCell="A476" sqref="A476"/>
     </sheetView>
   </sheetViews>

</xml_diff>